<commit_message>
docs: add live site link to README
</commit_message>
<xml_diff>
--- a/tools/2025 Racehorse Deaths (Active & Retired).xlsx
+++ b/tools/2025 Racehorse Deaths (Active & Retired).xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Racehorse-Memorial\tools\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E68EF57-1B07-4333-982E-5BA1DC19FC4A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F5687B6-1DE3-4510-92D8-914AD2646534}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21820" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -6885,9 +6885,9 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:Q223"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J10" sqref="J10"/>
+    <sheetView tabSelected="1" topLeftCell="Q1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="Q27" sqref="Q27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -8273,7 +8273,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="27" spans="1:17" ht="20" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:17" ht="40" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="1">
         <v>26</v>
       </c>
@@ -8322,7 +8322,7 @@
       <c r="P27" s="1" t="s">
         <v>284</v>
       </c>
-      <c r="Q27" s="1" t="s">
+      <c r="Q27" s="4" t="s">
         <v>1068</v>
       </c>
     </row>

</xml_diff>

<commit_message>
feat: Add image renaming tool and fix convert.py field preservation
- Add rename_images.py script to rename horse images based on JSON serial numbers
- Fix convert.py to properly preserve special fields (hasPhoto) by normalizing serial number types
- Rename 110 horse images to match JSON serial numbers for stable image paths
- Update README.md with project statistics (39 files, 7,703 lines of code)
- Add 5 new horse images (#66, #67, #68, #91, #02)
</commit_message>
<xml_diff>
--- a/tools/2025 Racehorse Deaths (Active & Retired).xlsx
+++ b/tools/2025 Racehorse Deaths (Active & Retired).xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Racehorse-Memorial\tools\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCB9619E-66A5-4587-BD1A-40ED09F50D92}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F78F98C2-7A0F-4594-B5C2-4571AB55BB1D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21820" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1537" uniqueCount="1098">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1600" uniqueCount="1131">
   <si>
     <t>序号</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -6483,6 +6483,307 @@
   </si>
   <si>
     <t>2012年新山纪念（G3）|2012年玫瑰锦标（G2）|2012年樱花赏（G1）|2012年优骏牝马（G1）|2012年秋华赏（G1）|2012·2013年日本杯（G1)|2014年迪拜司马经典赛（G1）|2014年有马纪念（G1）</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>日本</t>
+  </si>
+  <si>
+    <r>
+      <t>3岁未胜利比赛中，在通过第三弯道后因</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="楷体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>**左第3掌骨开放性骨折**</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="楷体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>（予后不良）中止比赛，</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="楷体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>**殒命赛场**</t>
+    </r>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>3岁以上1胜比赛中在第一弯道与前方马匹发生接触后跌倒后竞走中止，</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="楷体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>**右桡骨开放性骨折**</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="楷体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>（予后不良），</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="楷体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>**殒命赛场**</t>
+    </r>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>3岁以上1胜比赛中在第一弯道接触到跌倒的10号马ウマピョイ后跌倒，</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="楷体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>**左桡骨骨折**</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="楷体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>（预后不良），</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="楷体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>**殒命赛场**</t>
+    </r>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>仲秋S（3胜级）比赛中在最后直线路段中止比赛，</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="楷体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>**右第一指关节脱臼**</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="楷体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>（预后不良），</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="楷体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>**殒命赛场**</t>
+    </r>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>生涯首战3岁新马比赛中在第四弯道中止比赛，</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="楷体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>**左第三腕骨粉碎性骨折**</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="楷体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>（预后不良），</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="楷体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>**殒命赛场**</t>
+    </r>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>原因/事故|原因/脱臼|殒命赛场/平地</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>原因/事故|原因/骨折|殒命赛场/平地</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>アミドゥクール|Ami de Coeur</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>カハンガハンガ|Kahanga Hanga</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>呂宋火山</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Shamardal</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Kitten's Roar</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>ウマピョイ|Uma Pyoi</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>黄金伶人</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Sanitsu</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>22-3-7-4</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>1662万2000日圆</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>2024年C2二|2024年疾风！短跑者（C3）|2024年C2三</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>スティックバイミー|Stick By Me</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Molto Felice</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>10-1-1-0</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>1349万日元</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>2023年2岁新马</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>アロマデローサ|Aroma de Rosa</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Rose Whisper</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>劳动力</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>15-3-0-5</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>6740万5000日元</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>2022年2岁新马|2022年桔梗S（OP）|2025年西部体育日本赏（2胜级）</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>高情厚意</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Directa</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Anodin</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -6886,9 +7187,9 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:Q223"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="M1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="P39" sqref="P39"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A102" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F132" sqref="F132"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -12590,7 +12891,7 @@
         <v>1008</v>
       </c>
       <c r="M111" s="1" t="s">
-        <v>1042</v>
+        <v>1105</v>
       </c>
       <c r="N111" s="1" t="s">
         <v>842</v>
@@ -12649,7 +12950,7 @@
         <v>944</v>
       </c>
     </row>
-    <row r="113" spans="1:16" ht="20" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:17" ht="20" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A113" s="1">
         <v>112</v>
       </c>
@@ -12699,7 +13000,7 @@
         <v>943</v>
       </c>
     </row>
-    <row r="114" spans="1:16" ht="20" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:17" ht="20" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A114" s="1">
         <v>113</v>
       </c>
@@ -12737,7 +13038,7 @@
         <v>1011</v>
       </c>
       <c r="M114" s="1" t="s">
-        <v>1053</v>
+        <v>1104</v>
       </c>
       <c r="N114" s="1" t="s">
         <v>948</v>
@@ -12749,60 +13050,284 @@
         <v>950</v>
       </c>
     </row>
-    <row r="115" spans="1:16" ht="20" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D115" s="9"/>
-      <c r="E115" s="9"/>
-      <c r="P115" s="11"/>
-    </row>
-    <row r="116" spans="1:16" ht="20" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D116" s="9"/>
-      <c r="E116" s="9"/>
-    </row>
-    <row r="117" spans="1:16" ht="20" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D117" s="9"/>
-      <c r="E117" s="9"/>
-    </row>
-    <row r="118" spans="1:16" ht="20" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D118" s="9"/>
-      <c r="E118" s="9"/>
-    </row>
-    <row r="119" spans="1:16" ht="20" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D119" s="9"/>
-      <c r="E119" s="9"/>
-    </row>
-    <row r="120" spans="1:16" ht="20" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:17" ht="20" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A115" s="1">
+        <v>114</v>
+      </c>
+      <c r="B115" s="1" t="s">
+        <v>1107</v>
+      </c>
+      <c r="C115" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D115" s="9">
+        <v>44612</v>
+      </c>
+      <c r="E115" s="9">
+        <v>45830</v>
+      </c>
+      <c r="F115" s="1" t="s">
+        <v>1108</v>
+      </c>
+      <c r="G115" s="1" t="s">
+        <v>1109</v>
+      </c>
+      <c r="H115" s="1" t="s">
+        <v>1110</v>
+      </c>
+      <c r="I115" s="1" t="s">
+        <v>462</v>
+      </c>
+      <c r="J115" s="1" t="s">
+        <v>907</v>
+      </c>
+      <c r="K115" s="1" t="s">
+        <v>318</v>
+      </c>
+      <c r="L115" s="1" t="s">
+        <v>1099</v>
+      </c>
+      <c r="M115" s="1" t="s">
+        <v>1105</v>
+      </c>
+      <c r="N115" s="1" t="s">
+        <v>842</v>
+      </c>
+      <c r="O115" s="1" t="s">
+        <v>523</v>
+      </c>
+      <c r="Q115" s="11"/>
+    </row>
+    <row r="116" spans="1:17" ht="20" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A116" s="1">
+        <v>115</v>
+      </c>
+      <c r="B116" s="1" t="s">
+        <v>1111</v>
+      </c>
+      <c r="C116" s="1" t="s">
+        <v>1098</v>
+      </c>
+      <c r="D116" s="9">
+        <v>43866</v>
+      </c>
+      <c r="E116" s="9">
+        <v>45830</v>
+      </c>
+      <c r="F116" s="1" t="s">
+        <v>1112</v>
+      </c>
+      <c r="G116" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="H116" s="1" t="s">
+        <v>1113</v>
+      </c>
+      <c r="I116" s="1" t="s">
+        <v>854</v>
+      </c>
+      <c r="J116" s="1" t="s">
+        <v>907</v>
+      </c>
+      <c r="K116" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="L116" s="1" t="s">
+        <v>1100</v>
+      </c>
+      <c r="M116" s="1" t="s">
+        <v>1105</v>
+      </c>
+      <c r="N116" s="1" t="s">
+        <v>1114</v>
+      </c>
+      <c r="O116" s="1" t="s">
+        <v>1115</v>
+      </c>
+      <c r="P116" s="1" t="s">
+        <v>1116</v>
+      </c>
+    </row>
+    <row r="117" spans="1:17" ht="20" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A117" s="1">
+        <v>116</v>
+      </c>
+      <c r="B117" s="1" t="s">
+        <v>1117</v>
+      </c>
+      <c r="C117" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D117" s="9">
+        <v>44305</v>
+      </c>
+      <c r="E117" s="9">
+        <v>45830</v>
+      </c>
+      <c r="F117" s="1" t="s">
+        <v>878</v>
+      </c>
+      <c r="G117" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="H117" s="1" t="s">
+        <v>1118</v>
+      </c>
+      <c r="I117" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="J117" s="1" t="s">
+        <v>907</v>
+      </c>
+      <c r="K117" s="1" t="s">
+        <v>397</v>
+      </c>
+      <c r="L117" s="1" t="s">
+        <v>1101</v>
+      </c>
+      <c r="M117" s="1" t="s">
+        <v>1105</v>
+      </c>
+      <c r="N117" s="1" t="s">
+        <v>1119</v>
+      </c>
+      <c r="O117" s="1" t="s">
+        <v>1120</v>
+      </c>
+      <c r="P117" s="1" t="s">
+        <v>1121</v>
+      </c>
+    </row>
+    <row r="118" spans="1:17" ht="20" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A118" s="1">
+        <v>117</v>
+      </c>
+      <c r="B118" s="1" t="s">
+        <v>1122</v>
+      </c>
+      <c r="C118" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D118" s="9">
+        <v>43889</v>
+      </c>
+      <c r="E118" s="9">
+        <v>45914</v>
+      </c>
+      <c r="F118" s="1" t="s">
+        <v>859</v>
+      </c>
+      <c r="G118" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="H118" s="1" t="s">
+        <v>1123</v>
+      </c>
+      <c r="I118" s="1" t="s">
+        <v>1124</v>
+      </c>
+      <c r="J118" s="1" t="s">
+        <v>875</v>
+      </c>
+      <c r="K118" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="L118" s="1" t="s">
+        <v>1102</v>
+      </c>
+      <c r="M118" s="1" t="s">
+        <v>1104</v>
+      </c>
+      <c r="N118" s="1" t="s">
+        <v>1125</v>
+      </c>
+      <c r="O118" s="1" t="s">
+        <v>1126</v>
+      </c>
+      <c r="P118" s="1" t="s">
+        <v>1127</v>
+      </c>
+    </row>
+    <row r="119" spans="1:17" ht="20" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A119" s="1">
+        <v>118</v>
+      </c>
+      <c r="B119" s="1" t="s">
+        <v>1106</v>
+      </c>
+      <c r="C119" s="1" t="s">
+        <v>1098</v>
+      </c>
+      <c r="D119" s="9">
+        <v>44614</v>
+      </c>
+      <c r="E119" s="9">
+        <v>45662</v>
+      </c>
+      <c r="F119" s="1" t="s">
+        <v>1128</v>
+      </c>
+      <c r="G119" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="H119" s="1" t="s">
+        <v>1129</v>
+      </c>
+      <c r="I119" s="1" t="s">
+        <v>1130</v>
+      </c>
+      <c r="J119" s="1" t="s">
+        <v>520</v>
+      </c>
+      <c r="K119" s="1" t="s">
+        <v>521</v>
+      </c>
+      <c r="L119" s="1" t="s">
+        <v>1103</v>
+      </c>
+      <c r="M119" s="1" t="s">
+        <v>1105</v>
+      </c>
+      <c r="N119" s="1" t="s">
+        <v>522</v>
+      </c>
+      <c r="O119" s="1" t="s">
+        <v>523</v>
+      </c>
+    </row>
+    <row r="120" spans="1:17" ht="20" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D120" s="9"/>
       <c r="E120" s="9"/>
     </row>
-    <row r="121" spans="1:16" ht="20" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:17" ht="20" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D121" s="9"/>
       <c r="E121" s="9"/>
     </row>
-    <row r="122" spans="1:16" ht="20" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:17" ht="20" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D122" s="9"/>
       <c r="E122" s="9"/>
     </row>
-    <row r="123" spans="1:16" ht="20" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:17" ht="20" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D123" s="9"/>
       <c r="E123" s="9"/>
     </row>
-    <row r="124" spans="1:16" ht="20" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:17" ht="20" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D124" s="9"/>
       <c r="E124" s="9"/>
     </row>
-    <row r="125" spans="1:16" ht="20" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:17" ht="20" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D125" s="9"/>
       <c r="E125" s="9"/>
     </row>
-    <row r="126" spans="1:16" ht="20" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:17" ht="20" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D126" s="9"/>
       <c r="E126" s="9"/>
     </row>
-    <row r="127" spans="1:16" ht="20" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:17" ht="20" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D127" s="9"/>
       <c r="E127" s="9"/>
     </row>
-    <row r="128" spans="1:16" ht="20" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:17" ht="20" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D128" s="9"/>
       <c r="E128" s="9"/>
     </row>

</xml_diff>